<commit_message>
minor corrections service category added in FOC invoice
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Vendor_Settlement_Template-FoC-v4.xlsx
+++ b/application/controllers/excel-templates/Vendor_Settlement_Template-FoC-v4.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="59">
   <si>
     <t>Blackmelon Advance Technology Co. Pvt. Ltd.</t>
   </si>
@@ -198,6 +198,12 @@
   </si>
   <si>
     <t xml:space="preserve">247around Royalty %    </t>
+  </si>
+  <si>
+    <t>Service Category</t>
+  </si>
+  <si>
+    <t>{booking:price_tags}</t>
   </si>
 </sst>
 </file>
@@ -756,7 +762,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -921,6 +927,30 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -939,15 +969,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -998,18 +1019,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1029,14 +1038,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>290287</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>136072</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>200785</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>200784</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>150911</xdr:rowOff>
     </xdr:to>
@@ -1361,24 +1370,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="1" customWidth="1"/>
     <col min="3" max="3" width="8.6640625" customWidth="1"/>
-    <col min="5" max="5" width="9.5" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" customWidth="1"/>
-    <col min="7" max="8" width="9.1640625" customWidth="1"/>
-    <col min="9" max="9" width="9" customWidth="1"/>
-    <col min="10" max="11" width="9.1640625" customWidth="1"/>
+    <col min="5" max="6" width="9.5" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" customWidth="1"/>
+    <col min="8" max="9" width="9.1640625" customWidth="1"/>
+    <col min="10" max="10" width="9" customWidth="1"/>
+    <col min="11" max="12" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1390,8 +1399,9 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:11" ht="14" x14ac:dyDescent="0.2">
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:12" ht="14" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="22"/>
       <c r="C2" s="55" t="s">
@@ -1399,16 +1409,17 @@
       </c>
       <c r="D2" s="23"/>
       <c r="E2" s="24"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25" t="s">
+      <c r="F2" s="24"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="4"/>
+      <c r="I2" s="3"/>
       <c r="J2" s="4"/>
-      <c r="K2" s="5"/>
-    </row>
-    <row r="3" spans="1:11" ht="14" x14ac:dyDescent="0.2">
+      <c r="K2" s="4"/>
+      <c r="L2" s="5"/>
+    </row>
+    <row r="3" spans="1:12" ht="14" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="32" t="s">
         <v>30</v>
@@ -1418,46 +1429,49 @@
       </c>
       <c r="D3" s="27"/>
       <c r="E3" s="28"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29" t="s">
+      <c r="F3" s="28"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="7"/>
-      <c r="I3" s="6"/>
+      <c r="I3" s="7"/>
       <c r="J3" s="6"/>
-      <c r="K3" s="8"/>
-    </row>
-    <row r="4" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K3" s="6"/>
+      <c r="L3" s="8"/>
+    </row>
+    <row r="4" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="26"/>
-      <c r="C4" s="85" t="s">
+      <c r="C4" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="85"/>
-      <c r="E4" s="85"/>
-      <c r="F4" s="85"/>
-      <c r="G4" s="29" t="s">
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="7"/>
-      <c r="I4" s="6"/>
+      <c r="I4" s="7"/>
       <c r="J4" s="6"/>
-      <c r="K4" s="8"/>
-    </row>
-    <row r="5" spans="1:11" ht="14" x14ac:dyDescent="0.2">
+      <c r="K4" s="6"/>
+      <c r="L4" s="8"/>
+    </row>
+    <row r="5" spans="1:12" ht="14" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="26"/>
-      <c r="C5" s="85"/>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="6"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="28"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
-      <c r="K5" s="8"/>
-    </row>
-    <row r="6" spans="1:11" ht="14" x14ac:dyDescent="0.2">
+      <c r="K5" s="6"/>
+      <c r="L5" s="8"/>
+    </row>
+    <row r="6" spans="1:12" ht="14" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="32" t="s">
         <v>29</v>
@@ -1469,12 +1483,13 @@
       <c r="E6" s="28"/>
       <c r="F6" s="28"/>
       <c r="G6" s="28"/>
-      <c r="H6" s="6"/>
+      <c r="H6" s="28"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
-      <c r="K6" s="8"/>
-    </row>
-    <row r="7" spans="1:11" ht="14" x14ac:dyDescent="0.2">
+      <c r="K6" s="6"/>
+      <c r="L6" s="8"/>
+    </row>
+    <row r="7" spans="1:12" ht="14" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="26"/>
       <c r="C7" s="51" t="s">
@@ -1484,12 +1499,13 @@
       <c r="E7" s="28"/>
       <c r="F7" s="28"/>
       <c r="G7" s="28"/>
-      <c r="H7" s="6"/>
+      <c r="H7" s="28"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
-      <c r="K7" s="8"/>
-    </row>
-    <row r="8" spans="1:11" ht="14" x14ac:dyDescent="0.2">
+      <c r="K7" s="6"/>
+      <c r="L7" s="8"/>
+    </row>
+    <row r="8" spans="1:12" ht="14" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="30"/>
       <c r="C8" s="51" t="s">
@@ -1499,12 +1515,13 @@
       <c r="E8" s="28"/>
       <c r="F8" s="28"/>
       <c r="G8" s="28"/>
-      <c r="H8" s="6"/>
+      <c r="H8" s="28"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
-      <c r="K8" s="8"/>
-    </row>
-    <row r="9" spans="1:11" ht="14" x14ac:dyDescent="0.2">
+      <c r="K8" s="6"/>
+      <c r="L8" s="8"/>
+    </row>
+    <row r="9" spans="1:12" ht="14" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="32"/>
       <c r="C9" s="52" t="s">
@@ -1514,12 +1531,13 @@
       <c r="E9" s="28"/>
       <c r="F9" s="28"/>
       <c r="G9" s="28"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="6"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="10"/>
       <c r="J9" s="6"/>
-      <c r="K9" s="8"/>
-    </row>
-    <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K9" s="6"/>
+      <c r="L9" s="8"/>
+    </row>
+    <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="34"/>
       <c r="C10" s="52" t="s">
@@ -1529,12 +1547,13 @@
       <c r="E10" s="36"/>
       <c r="F10" s="36"/>
       <c r="G10" s="36"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="13"/>
-    </row>
-    <row r="11" spans="1:11" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H10" s="36"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="13"/>
+    </row>
+    <row r="11" spans="1:12" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="18" t="s">
         <v>3</v>
@@ -1549,25 +1568,28 @@
         <v>5</v>
       </c>
       <c r="F11" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="G11" s="20" t="s">
+      <c r="H11" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H11" s="20" t="s">
+      <c r="I11" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="I11" s="20" t="s">
+      <c r="J11" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="20" t="s">
+      <c r="K11" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="K11" s="21" t="s">
+      <c r="L11" s="21" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9"/>
       <c r="B12" s="15" t="s">
         <v>11</v>
@@ -1582,25 +1604,28 @@
         <v>14</v>
       </c>
       <c r="F12" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="G12" s="16" t="s">
+      <c r="H12" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="H12" s="16" t="s">
+      <c r="I12" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="I12" s="16" t="s">
+      <c r="J12" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J12" s="16" t="s">
+      <c r="K12" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="K12" s="17" t="s">
+      <c r="L12" s="17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="14" x14ac:dyDescent="0.2">
       <c r="A13" s="9"/>
       <c r="B13" s="14"/>
       <c r="C13" s="6"/>
@@ -1611,96 +1636,99 @@
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
-      <c r="K13" s="8"/>
-    </row>
-    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K13" s="6"/>
+      <c r="L13" s="8"/>
+    </row>
+    <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
-      <c r="B14" s="59" t="s">
+      <c r="B14" s="67" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="60"/>
-      <c r="D14" s="60"/>
-      <c r="E14" s="60"/>
-      <c r="F14" s="60"/>
-      <c r="G14" s="60"/>
-      <c r="H14" s="60"/>
-      <c r="I14" s="60"/>
-      <c r="J14" s="60"/>
-      <c r="K14" s="61"/>
-    </row>
-    <row r="15" spans="1:11" ht="65" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="68"/>
+      <c r="D14" s="68"/>
+      <c r="E14" s="68"/>
+      <c r="F14" s="68"/>
+      <c r="G14" s="68"/>
+      <c r="H14" s="68"/>
+      <c r="I14" s="68"/>
+      <c r="J14" s="68"/>
+      <c r="K14" s="68"/>
+      <c r="L14" s="69"/>
+    </row>
+    <row r="15" spans="1:12" ht="65" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
-      <c r="B15" s="56" t="s">
+      <c r="B15" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="57"/>
-      <c r="G15" s="57"/>
-      <c r="H15" s="57"/>
-      <c r="I15" s="57"/>
-      <c r="J15" s="57"/>
-      <c r="K15" s="58"/>
-    </row>
-    <row r="16" spans="1:11" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="65"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="65"/>
+      <c r="I15" s="65"/>
+      <c r="J15" s="65"/>
+      <c r="K15" s="65"/>
+      <c r="L15" s="66"/>
+    </row>
+    <row r="16" spans="1:12" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
-      <c r="B16" s="64"/>
-      <c r="C16" s="64"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="64"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="38" t="s">
+      <c r="B16" s="62"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="62"/>
+      <c r="E16" s="62"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="H16" s="39" t="s">
+      <c r="I16" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="I16" s="39" t="s">
+      <c r="J16" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="J16" s="39" t="s">
+      <c r="K16" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="K16" s="40" t="s">
+      <c r="L16" s="40" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
-      <c r="B17" s="73"/>
-      <c r="C17" s="74"/>
-      <c r="D17" s="74"/>
-      <c r="E17" s="74"/>
-      <c r="F17" s="75"/>
-      <c r="G17" s="41" t="s">
+      <c r="B17" s="78"/>
+      <c r="C17" s="79"/>
+      <c r="D17" s="79"/>
+      <c r="E17" s="79"/>
+      <c r="F17" s="79"/>
+      <c r="G17" s="80"/>
+      <c r="H17" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="H17" s="42" t="s">
+      <c r="I17" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="I17" s="43" t="s">
+      <c r="J17" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="J17" s="43" t="s">
+      <c r="K17" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="K17" s="46" t="s">
+      <c r="L17" s="46" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
-      <c r="B18" s="70" t="s">
+      <c r="B18" s="75" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="71"/>
-      <c r="D18" s="71"/>
-      <c r="E18" s="71"/>
-      <c r="F18" s="72"/>
-      <c r="G18" s="44">
-        <v>0.3</v>
-      </c>
+      <c r="C18" s="76"/>
+      <c r="D18" s="76"/>
+      <c r="E18" s="76"/>
+      <c r="F18" s="76"/>
+      <c r="G18" s="77"/>
       <c r="H18" s="44">
         <v>0.3</v>
       </c>
@@ -1710,182 +1738,194 @@
       <c r="J18" s="44">
         <v>0.3</v>
       </c>
-      <c r="K18" s="46"/>
-    </row>
-    <row r="19" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K18" s="44">
+        <v>0.3</v>
+      </c>
+      <c r="L18" s="46"/>
+    </row>
+    <row r="19" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
-      <c r="B19" s="70" t="s">
+      <c r="B19" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="71"/>
-      <c r="D19" s="71"/>
-      <c r="E19" s="71"/>
-      <c r="F19" s="72"/>
-      <c r="G19" s="41" t="s">
+      <c r="C19" s="76"/>
+      <c r="D19" s="76"/>
+      <c r="E19" s="76"/>
+      <c r="F19" s="76"/>
+      <c r="G19" s="77"/>
+      <c r="H19" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="H19" s="47" t="s">
+      <c r="I19" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="I19" s="45" t="s">
+      <c r="J19" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="J19" s="45" t="s">
+      <c r="K19" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="K19" s="46"/>
-    </row>
-    <row r="20" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L19" s="46"/>
+    </row>
+    <row r="20" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
-      <c r="B20" s="70" t="s">
+      <c r="B20" s="75" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="71"/>
-      <c r="D20" s="71"/>
-      <c r="E20" s="71"/>
-      <c r="F20" s="72"/>
-      <c r="G20" s="82" t="s">
+      <c r="C20" s="76"/>
+      <c r="D20" s="76"/>
+      <c r="E20" s="76"/>
+      <c r="F20" s="76"/>
+      <c r="G20" s="77"/>
+      <c r="H20" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="H20" s="83"/>
-      <c r="I20" s="83"/>
-      <c r="J20" s="83"/>
-      <c r="K20" s="84"/>
-    </row>
-    <row r="21" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I20" s="58"/>
+      <c r="J20" s="58"/>
+      <c r="K20" s="58"/>
+      <c r="L20" s="59"/>
+    </row>
+    <row r="21" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
-      <c r="B21" s="79"/>
-      <c r="C21" s="80"/>
-      <c r="D21" s="80"/>
-      <c r="E21" s="80"/>
-      <c r="F21" s="81"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="50"/>
-      <c r="I21" s="24"/>
+      <c r="B21" s="84"/>
+      <c r="C21" s="85"/>
+      <c r="D21" s="85"/>
+      <c r="E21" s="85"/>
+      <c r="F21" s="85"/>
+      <c r="G21" s="86"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="50"/>
       <c r="J21" s="24"/>
-      <c r="K21" s="48"/>
-      <c r="L21" s="49"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="48"/>
       <c r="M21" s="49"/>
-    </row>
-    <row r="22" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="N21" s="49"/>
+    </row>
+    <row r="22" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
-      <c r="B22" s="76"/>
-      <c r="C22" s="77"/>
-      <c r="D22" s="77"/>
-      <c r="E22" s="77"/>
-      <c r="F22" s="77"/>
-      <c r="G22" s="77"/>
-      <c r="H22" s="77"/>
-      <c r="I22" s="77"/>
-      <c r="J22" s="77"/>
-      <c r="K22" s="78"/>
-    </row>
-    <row r="23" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="81"/>
+      <c r="C22" s="82"/>
+      <c r="D22" s="82"/>
+      <c r="E22" s="82"/>
+      <c r="F22" s="82"/>
+      <c r="G22" s="82"/>
+      <c r="H22" s="82"/>
+      <c r="I22" s="82"/>
+      <c r="J22" s="82"/>
+      <c r="K22" s="82"/>
+      <c r="L22" s="83"/>
+    </row>
+    <row r="23" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
-      <c r="B23" s="67" t="s">
+      <c r="B23" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="68"/>
-      <c r="D23" s="68"/>
-      <c r="E23" s="68"/>
-      <c r="F23" s="68"/>
-      <c r="G23" s="68"/>
-      <c r="H23" s="68"/>
-      <c r="I23" s="68"/>
-      <c r="J23" s="68"/>
-      <c r="K23" s="69"/>
-    </row>
-    <row r="24" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="73"/>
+      <c r="D23" s="73"/>
+      <c r="E23" s="73"/>
+      <c r="F23" s="73"/>
+      <c r="G23" s="73"/>
+      <c r="H23" s="73"/>
+      <c r="I23" s="73"/>
+      <c r="J23" s="73"/>
+      <c r="K23" s="73"/>
+      <c r="L23" s="74"/>
+    </row>
+    <row r="24" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
-      <c r="B24" s="62" t="s">
+      <c r="B24" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="63"/>
-      <c r="D24" s="63"/>
-      <c r="E24" s="65" t="s">
+      <c r="C24" s="61"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="70" t="s">
         <v>50</v>
       </c>
-      <c r="F24" s="65"/>
-      <c r="G24" s="65"/>
-      <c r="H24" s="65"/>
-      <c r="I24" s="65"/>
-      <c r="J24" s="65"/>
-      <c r="K24" s="65"/>
-    </row>
-    <row r="25" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F24" s="70"/>
+      <c r="G24" s="70"/>
+      <c r="H24" s="70"/>
+      <c r="I24" s="70"/>
+      <c r="J24" s="70"/>
+      <c r="K24" s="70"/>
+      <c r="L24" s="70"/>
+    </row>
+    <row r="25" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
-      <c r="B25" s="62" t="s">
+      <c r="B25" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="64"/>
-      <c r="D25" s="64"/>
-      <c r="E25" s="66" t="s">
+      <c r="C25" s="62"/>
+      <c r="D25" s="62"/>
+      <c r="E25" s="71" t="s">
         <v>51</v>
       </c>
-      <c r="F25" s="66"/>
-      <c r="G25" s="66"/>
-      <c r="H25" s="66"/>
-      <c r="I25" s="66"/>
-      <c r="J25" s="66"/>
-      <c r="K25" s="66"/>
-    </row>
-    <row r="26" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F25" s="71"/>
+      <c r="G25" s="71"/>
+      <c r="H25" s="71"/>
+      <c r="I25" s="71"/>
+      <c r="J25" s="71"/>
+      <c r="K25" s="71"/>
+      <c r="L25" s="71"/>
+    </row>
+    <row r="26" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
-      <c r="B26" s="62" t="s">
+      <c r="B26" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="64"/>
-      <c r="D26" s="64"/>
-      <c r="E26" s="65" t="s">
+      <c r="C26" s="62"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="70" t="s">
         <v>52</v>
       </c>
-      <c r="F26" s="65"/>
-      <c r="G26" s="65"/>
-      <c r="H26" s="65"/>
-      <c r="I26" s="65"/>
-      <c r="J26" s="65"/>
-      <c r="K26" s="65"/>
-    </row>
-    <row r="27" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F26" s="70"/>
+      <c r="G26" s="70"/>
+      <c r="H26" s="70"/>
+      <c r="I26" s="70"/>
+      <c r="J26" s="70"/>
+      <c r="K26" s="70"/>
+      <c r="L26" s="70"/>
+    </row>
+    <row r="27" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
-      <c r="B27" s="62" t="s">
+      <c r="B27" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="63"/>
-      <c r="D27" s="63"/>
-      <c r="E27" s="65" t="s">
+      <c r="C27" s="61"/>
+      <c r="D27" s="61"/>
+      <c r="E27" s="70" t="s">
         <v>53</v>
       </c>
-      <c r="F27" s="65"/>
-      <c r="G27" s="65"/>
-      <c r="H27" s="65"/>
-      <c r="I27" s="65"/>
-      <c r="J27" s="65"/>
-      <c r="K27" s="65"/>
+      <c r="F27" s="70"/>
+      <c r="G27" s="70"/>
+      <c r="H27" s="70"/>
+      <c r="I27" s="70"/>
+      <c r="J27" s="70"/>
+      <c r="K27" s="70"/>
+      <c r="L27" s="70"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="20">
-    <mergeCell ref="G20:K20"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="C4:F5"/>
-    <mergeCell ref="B15:K15"/>
-    <mergeCell ref="B14:K14"/>
     <mergeCell ref="B27:D27"/>
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="B25:D25"/>
-    <mergeCell ref="E27:K27"/>
-    <mergeCell ref="E26:K26"/>
-    <mergeCell ref="E25:K25"/>
-    <mergeCell ref="E24:K24"/>
-    <mergeCell ref="B23:K23"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B22:K22"/>
-    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="E27:L27"/>
+    <mergeCell ref="E26:L26"/>
+    <mergeCell ref="E25:L25"/>
+    <mergeCell ref="H20:L20"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="C4:G5"/>
+    <mergeCell ref="B15:L15"/>
+    <mergeCell ref="B14:L14"/>
+    <mergeCell ref="E24:L24"/>
+    <mergeCell ref="B23:L23"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B22:L22"/>
+    <mergeCell ref="B21:G21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Around royalty component removed from Vendor FOC invoices
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Vendor_Settlement_Template-FoC-v4.xlsx
+++ b/application/controllers/excel-templates/Vendor_Settlement_Template-FoC-v4.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="61">
   <si>
     <t>Blackmelon Advance Technology Co. Pvt. Ltd.</t>
   </si>
@@ -95,9 +95,6 @@
     <t>{meta:msg}</t>
   </si>
   <si>
-    <t xml:space="preserve">247around Royality Breakup    </t>
-  </si>
-  <si>
     <t>Appliance</t>
   </si>
   <si>
@@ -113,9 +110,6 @@
     <t>Beneficiary Bank Name &amp; Address</t>
   </si>
   <si>
-    <t>{meta:r_st}</t>
-  </si>
-  <si>
     <t>To:</t>
   </si>
   <si>
@@ -164,21 +158,9 @@
     <t>{meta:t_total}</t>
   </si>
   <si>
-    <t>{meta:r_ic}</t>
-  </si>
-  <si>
-    <t>{meta:r_stand}</t>
-  </si>
-  <si>
-    <t>{meta:r_vat}</t>
-  </si>
-  <si>
     <t xml:space="preserve">Amount To Be Paid By 247around    </t>
   </si>
   <si>
-    <t>{meta:t_vp}</t>
-  </si>
-  <si>
     <t>{meta:beneficiary_name}</t>
   </si>
   <si>
@@ -197,9 +179,6 @@
     <t>Royalty Invoice</t>
   </si>
   <si>
-    <t xml:space="preserve">247around Royalty %    </t>
-  </si>
-  <si>
     <t>Service Category</t>
   </si>
   <si>
@@ -216,13 +195,28 @@
   </si>
   <si>
     <t>{booking:appliance_capacity}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Net Amount To Be Paid By 247around    </t>
+  </si>
+  <si>
+    <t>{meta:tds}</t>
+  </si>
+  <si>
+    <t>{meta:t_vp_wo_tds}</t>
+  </si>
+  <si>
+    <t>{meta:t_vp_w_tds}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tax Deducted @ 10%    </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -259,14 +253,8 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -282,14 +270,8 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="40">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -472,49 +454,177 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="thin">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color rgb="FF000000"/>
       </left>
       <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -526,9 +636,7 @@
       <top style="medium">
         <color auto="1"/>
       </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -537,9 +645,7 @@
       <top style="medium">
         <color auto="1"/>
       </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -550,9 +656,18 @@
       <top style="medium">
         <color auto="1"/>
       </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -563,24 +678,7 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -588,193 +686,19 @@
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
       <top style="medium">
         <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -884,43 +808,19 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="7" fillId="4" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -936,54 +836,48 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -992,44 +886,50 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1384,8 +1284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1418,7 +1318,7 @@
     <row r="2" spans="1:14" ht="14" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="22"/>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="46" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="23"/>
@@ -1438,9 +1338,9 @@
     <row r="3" spans="1:14" ht="14" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="53" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="45" t="s">
         <v>16</v>
       </c>
       <c r="D3" s="27"/>
@@ -1460,15 +1360,15 @@
     <row r="4" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="26"/>
-      <c r="C4" s="63" t="s">
+      <c r="C4" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
-      <c r="G4" s="63"/>
-      <c r="H4" s="63"/>
-      <c r="I4" s="63"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
       <c r="J4" s="29" t="s">
         <v>20</v>
       </c>
@@ -1480,13 +1380,13 @@
     <row r="5" spans="1:14" ht="14" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="26"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="63"/>
-      <c r="H5" s="63"/>
-      <c r="I5" s="63"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="54"/>
       <c r="J5" s="28"/>
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
@@ -1496,9 +1396,9 @@
     <row r="6" spans="1:14" ht="14" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="52" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="44" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="27"/>
@@ -1516,7 +1416,7 @@
     <row r="7" spans="1:14" ht="14" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="26"/>
-      <c r="C7" s="50" t="s">
+      <c r="C7" s="42" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="27"/>
@@ -1534,7 +1434,7 @@
     <row r="8" spans="1:14" ht="14" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="30"/>
-      <c r="C8" s="50" t="s">
+      <c r="C8" s="42" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="31"/>
@@ -1552,7 +1452,7 @@
     <row r="9" spans="1:14" ht="14" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="32"/>
-      <c r="C9" s="51" t="s">
+      <c r="C9" s="43" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="33"/>
@@ -1570,7 +1470,7 @@
     <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="34"/>
-      <c r="C10" s="51" t="s">
+      <c r="C10" s="43" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="35"/>
@@ -1594,34 +1494,34 @@
         <v>4</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="G11" s="20" t="s">
         <v>5</v>
       </c>
       <c r="H11" s="20" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="I11" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J11" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="K11" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="J11" s="20" t="s">
+      <c r="L11" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="K11" s="20" t="s">
+      <c r="M11" s="20" t="s">
         <v>33</v>
-      </c>
-      <c r="L11" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="M11" s="20" t="s">
-        <v>35</v>
       </c>
       <c r="N11" s="21" t="s">
         <v>6</v>
@@ -1639,34 +1539,34 @@
         <v>13</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="G12" s="16" t="s">
         <v>14</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="I12" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="J12" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="K12" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="J12" s="16" t="s">
+      <c r="L12" s="16" t="s">
         <v>37</v>
-      </c>
-      <c r="K12" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="L12" s="16" t="s">
-        <v>39</v>
       </c>
       <c r="M12" s="16" t="s">
         <v>15</v>
       </c>
       <c r="N12" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="14" x14ac:dyDescent="0.2">
@@ -1687,305 +1587,288 @@
     </row>
     <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
-      <c r="B14" s="67" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="68"/>
-      <c r="D14" s="68"/>
-      <c r="E14" s="68"/>
-      <c r="F14" s="68"/>
-      <c r="G14" s="68"/>
-      <c r="H14" s="68"/>
-      <c r="I14" s="68"/>
-      <c r="J14" s="68"/>
-      <c r="K14" s="68"/>
-      <c r="L14" s="68"/>
-      <c r="M14" s="68"/>
-      <c r="N14" s="69"/>
+      <c r="B14" s="58" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="59"/>
+      <c r="H14" s="59"/>
+      <c r="I14" s="59"/>
+      <c r="J14" s="59"/>
+      <c r="K14" s="59"/>
+      <c r="L14" s="59"/>
+      <c r="M14" s="59"/>
+      <c r="N14" s="60"/>
     </row>
     <row r="15" spans="1:14" ht="65" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
-      <c r="B15" s="64" t="s">
+      <c r="B15" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="65"/>
-      <c r="D15" s="65"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="65"/>
-      <c r="G15" s="65"/>
-      <c r="H15" s="65"/>
-      <c r="I15" s="65"/>
-      <c r="J15" s="65"/>
-      <c r="K15" s="65"/>
-      <c r="L15" s="65"/>
-      <c r="M15" s="65"/>
-      <c r="N15" s="66"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="56"/>
+      <c r="I15" s="56"/>
+      <c r="J15" s="56"/>
+      <c r="K15" s="56"/>
+      <c r="L15" s="56"/>
+      <c r="M15" s="56"/>
+      <c r="N15" s="57"/>
     </row>
     <row r="16" spans="1:14" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
-      <c r="B16" s="77"/>
-      <c r="C16" s="78"/>
-      <c r="D16" s="78"/>
-      <c r="E16" s="78"/>
-      <c r="F16" s="78"/>
-      <c r="G16" s="78"/>
-      <c r="H16" s="78"/>
-      <c r="I16" s="79"/>
+      <c r="B16" s="67"/>
+      <c r="C16" s="68"/>
+      <c r="D16" s="68"/>
+      <c r="E16" s="68"/>
+      <c r="F16" s="68"/>
+      <c r="G16" s="68"/>
+      <c r="H16" s="68"/>
+      <c r="I16" s="69"/>
       <c r="J16" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="K16" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="L16" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="K16" s="38" t="s">
+      <c r="M16" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="L16" s="38" t="s">
+      <c r="N16" s="39" t="s">
         <v>33</v>
-      </c>
-      <c r="M16" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="N16" s="39" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
-      <c r="B17" s="77"/>
-      <c r="C17" s="78"/>
-      <c r="D17" s="78"/>
-      <c r="E17" s="78"/>
-      <c r="F17" s="78"/>
-      <c r="G17" s="78"/>
-      <c r="H17" s="78"/>
-      <c r="I17" s="79"/>
-      <c r="J17" s="40" t="s">
+      <c r="B17" s="67"/>
+      <c r="C17" s="68"/>
+      <c r="D17" s="68"/>
+      <c r="E17" s="68"/>
+      <c r="F17" s="68"/>
+      <c r="G17" s="68"/>
+      <c r="H17" s="68"/>
+      <c r="I17" s="69"/>
+      <c r="J17" s="76" t="s">
+        <v>38</v>
+      </c>
+      <c r="K17" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="L17" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="K17" s="41" t="s">
+      <c r="M17" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="L17" s="42" t="s">
+      <c r="N17" s="77" t="s">
         <v>42</v>
-      </c>
-      <c r="M17" s="42" t="s">
-        <v>43</v>
-      </c>
-      <c r="N17" s="45" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
-      <c r="B18" s="74" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" s="75"/>
-      <c r="D18" s="75"/>
-      <c r="E18" s="75"/>
-      <c r="F18" s="75"/>
-      <c r="G18" s="75"/>
-      <c r="H18" s="75"/>
-      <c r="I18" s="76"/>
-      <c r="J18" s="43">
-        <v>0.3</v>
-      </c>
-      <c r="K18" s="43">
-        <v>0.3</v>
-      </c>
-      <c r="L18" s="43">
-        <v>0.3</v>
-      </c>
-      <c r="M18" s="43">
-        <v>0.3</v>
-      </c>
-      <c r="N18" s="45"/>
+      <c r="B18" s="64" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="65"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="65"/>
+      <c r="F18" s="65"/>
+      <c r="G18" s="65"/>
+      <c r="H18" s="65"/>
+      <c r="I18" s="66"/>
+      <c r="J18" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="K18" s="52"/>
+      <c r="L18" s="52"/>
+      <c r="M18" s="52"/>
+      <c r="N18" s="52"/>
     </row>
     <row r="19" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
-      <c r="B19" s="74" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="75"/>
-      <c r="D19" s="75"/>
-      <c r="E19" s="75"/>
-      <c r="F19" s="75"/>
-      <c r="G19" s="75"/>
-      <c r="H19" s="75"/>
-      <c r="I19" s="76"/>
-      <c r="J19" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="K19" s="46" t="s">
-        <v>28</v>
-      </c>
-      <c r="L19" s="44" t="s">
-        <v>46</v>
-      </c>
-      <c r="M19" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="N19" s="45"/>
+      <c r="B19" s="64" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="65"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="65"/>
+      <c r="F19" s="65"/>
+      <c r="G19" s="65"/>
+      <c r="H19" s="65"/>
+      <c r="I19" s="66"/>
+      <c r="J19" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="K19" s="52"/>
+      <c r="L19" s="52"/>
+      <c r="M19" s="52"/>
+      <c r="N19" s="52"/>
     </row>
     <row r="20" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
-      <c r="B20" s="74" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" s="75"/>
-      <c r="D20" s="75"/>
-      <c r="E20" s="75"/>
-      <c r="F20" s="75"/>
-      <c r="G20" s="75"/>
-      <c r="H20" s="75"/>
-      <c r="I20" s="76"/>
-      <c r="J20" s="57" t="s">
-        <v>49</v>
-      </c>
-      <c r="K20" s="58"/>
-      <c r="L20" s="58"/>
-      <c r="M20" s="58"/>
-      <c r="N20" s="59"/>
+      <c r="B20" s="64" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="65"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="65"/>
+      <c r="F20" s="65"/>
+      <c r="G20" s="65"/>
+      <c r="H20" s="65"/>
+      <c r="I20" s="66"/>
+      <c r="J20" s="49" t="s">
+        <v>59</v>
+      </c>
+      <c r="K20" s="49"/>
+      <c r="L20" s="49"/>
+      <c r="M20" s="49"/>
+      <c r="N20" s="49"/>
     </row>
     <row r="21" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
-      <c r="B21" s="83"/>
-      <c r="C21" s="84"/>
-      <c r="D21" s="84"/>
-      <c r="E21" s="84"/>
-      <c r="F21" s="84"/>
-      <c r="G21" s="84"/>
-      <c r="H21" s="84"/>
-      <c r="I21" s="85"/>
-      <c r="J21" s="24"/>
-      <c r="K21" s="49"/>
-      <c r="L21" s="24"/>
-      <c r="M21" s="24"/>
-      <c r="N21" s="47"/>
-      <c r="O21" s="48"/>
-      <c r="P21" s="48"/>
+      <c r="B21" s="73"/>
+      <c r="C21" s="74"/>
+      <c r="D21" s="74"/>
+      <c r="E21" s="74"/>
+      <c r="F21" s="74"/>
+      <c r="G21" s="74"/>
+      <c r="H21" s="74"/>
+      <c r="I21" s="75"/>
+      <c r="J21" s="70"/>
+      <c r="K21" s="71"/>
+      <c r="L21" s="71"/>
+      <c r="M21" s="71"/>
+      <c r="N21" s="78"/>
+      <c r="O21" s="41"/>
+      <c r="P21" s="41"/>
     </row>
     <row r="22" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
-      <c r="B22" s="80"/>
-      <c r="C22" s="81"/>
-      <c r="D22" s="81"/>
-      <c r="E22" s="81"/>
-      <c r="F22" s="81"/>
-      <c r="G22" s="81"/>
-      <c r="H22" s="81"/>
-      <c r="I22" s="81"/>
-      <c r="J22" s="81"/>
-      <c r="K22" s="81"/>
-      <c r="L22" s="81"/>
-      <c r="M22" s="81"/>
-      <c r="N22" s="82"/>
+      <c r="B22" s="70"/>
+      <c r="C22" s="71"/>
+      <c r="D22" s="71"/>
+      <c r="E22" s="71"/>
+      <c r="F22" s="71"/>
+      <c r="G22" s="71"/>
+      <c r="H22" s="71"/>
+      <c r="I22" s="71"/>
+      <c r="J22" s="71"/>
+      <c r="K22" s="71"/>
+      <c r="L22" s="71"/>
+      <c r="M22" s="71"/>
+      <c r="N22" s="72"/>
     </row>
     <row r="23" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
-      <c r="B23" s="71" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" s="72"/>
-      <c r="D23" s="72"/>
-      <c r="E23" s="72"/>
-      <c r="F23" s="72"/>
-      <c r="G23" s="72"/>
-      <c r="H23" s="72"/>
-      <c r="I23" s="72"/>
-      <c r="J23" s="72"/>
-      <c r="K23" s="72"/>
-      <c r="L23" s="72"/>
-      <c r="M23" s="72"/>
-      <c r="N23" s="73"/>
+      <c r="B23" s="61" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="62"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="62"/>
+      <c r="G23" s="62"/>
+      <c r="H23" s="62"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="62"/>
+      <c r="K23" s="62"/>
+      <c r="L23" s="62"/>
+      <c r="M23" s="62"/>
+      <c r="N23" s="63"/>
     </row>
     <row r="24" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
-      <c r="B24" s="60" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="61"/>
-      <c r="D24" s="61"/>
-      <c r="E24" s="55"/>
-      <c r="F24" s="55"/>
-      <c r="G24" s="70" t="s">
-        <v>50</v>
-      </c>
-      <c r="H24" s="70"/>
-      <c r="I24" s="70"/>
-      <c r="J24" s="70"/>
-      <c r="K24" s="70"/>
-      <c r="L24" s="70"/>
-      <c r="M24" s="70"/>
-      <c r="N24" s="70"/>
+      <c r="B24" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="50"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="H24" s="52"/>
+      <c r="I24" s="52"/>
+      <c r="J24" s="52"/>
+      <c r="K24" s="52"/>
+      <c r="L24" s="52"/>
+      <c r="M24" s="52"/>
+      <c r="N24" s="52"/>
     </row>
     <row r="25" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
-      <c r="B25" s="60" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="62"/>
-      <c r="D25" s="62"/>
-      <c r="E25" s="56"/>
-      <c r="F25" s="56"/>
-      <c r="G25" s="86" t="s">
-        <v>51</v>
-      </c>
-      <c r="H25" s="86"/>
-      <c r="I25" s="86"/>
-      <c r="J25" s="86"/>
-      <c r="K25" s="86"/>
-      <c r="L25" s="86"/>
-      <c r="M25" s="86"/>
-      <c r="N25" s="86"/>
+      <c r="B25" s="49" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="51"/>
+      <c r="D25" s="51"/>
+      <c r="E25" s="48"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="53" t="s">
+        <v>45</v>
+      </c>
+      <c r="H25" s="53"/>
+      <c r="I25" s="53"/>
+      <c r="J25" s="53"/>
+      <c r="K25" s="53"/>
+      <c r="L25" s="53"/>
+      <c r="M25" s="53"/>
+      <c r="N25" s="53"/>
     </row>
     <row r="26" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
-      <c r="B26" s="60" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="62"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="56"/>
-      <c r="F26" s="56"/>
-      <c r="G26" s="70" t="s">
-        <v>52</v>
-      </c>
-      <c r="H26" s="70"/>
-      <c r="I26" s="70"/>
-      <c r="J26" s="70"/>
-      <c r="K26" s="70"/>
-      <c r="L26" s="70"/>
-      <c r="M26" s="70"/>
-      <c r="N26" s="70"/>
+      <c r="B26" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="51"/>
+      <c r="D26" s="51"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="48"/>
+      <c r="G26" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="H26" s="52"/>
+      <c r="I26" s="52"/>
+      <c r="J26" s="52"/>
+      <c r="K26" s="52"/>
+      <c r="L26" s="52"/>
+      <c r="M26" s="52"/>
+      <c r="N26" s="52"/>
     </row>
     <row r="27" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
-      <c r="B27" s="60" t="s">
+      <c r="B27" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="61"/>
-      <c r="D27" s="61"/>
-      <c r="E27" s="55"/>
-      <c r="F27" s="55"/>
-      <c r="G27" s="70" t="s">
-        <v>53</v>
-      </c>
-      <c r="H27" s="70"/>
-      <c r="I27" s="70"/>
-      <c r="J27" s="70"/>
-      <c r="K27" s="70"/>
-      <c r="L27" s="70"/>
-      <c r="M27" s="70"/>
-      <c r="N27" s="70"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H27" s="52"/>
+      <c r="I27" s="52"/>
+      <c r="J27" s="52"/>
+      <c r="K27" s="52"/>
+      <c r="L27" s="52"/>
+      <c r="M27" s="52"/>
+      <c r="N27" s="52"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <mergeCells count="20">
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="G27:N27"/>
-    <mergeCell ref="G26:N26"/>
-    <mergeCell ref="G25:N25"/>
+  <mergeCells count="23">
+    <mergeCell ref="J21:N21"/>
     <mergeCell ref="J20:N20"/>
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="C4:I5"/>
@@ -2000,6 +1883,14 @@
     <mergeCell ref="B22:N22"/>
     <mergeCell ref="B21:I21"/>
     <mergeCell ref="B16:I16"/>
+    <mergeCell ref="J18:N18"/>
+    <mergeCell ref="J19:N19"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="G27:N27"/>
+    <mergeCell ref="G26:N26"/>
+    <mergeCell ref="G25:N25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Minor correction in template
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Vendor_Settlement_Template-FoC-v4.xlsx
+++ b/application/controllers/excel-templates/Vendor_Settlement_Template-FoC-v4.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anujaggarwal/Downloads/templates/anuj/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/247around-adminp-aws/application/controllers/excel-templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -337,7 +337,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -440,21 +440,6 @@
       <left style="medium">
         <color auto="1"/>
       </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
       <right/>
       <top style="thin">
         <color auto="1"/>
@@ -632,7 +617,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -688,10 +673,10 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -706,22 +691,22 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -730,16 +715,16 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -754,10 +739,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -766,116 +751,122 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1156,8 +1147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34:N34"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26:N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1192,21 +1183,21 @@
     </row>
     <row r="2" spans="1:14" ht="18" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="58"/>
-      <c r="N2" s="58"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="64"/>
+      <c r="M2" s="64"/>
+      <c r="N2" s="64"/>
     </row>
     <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
@@ -1446,21 +1437,21 @@
     </row>
     <row r="16" spans="1:14" ht="16" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
-      <c r="B16" s="61" t="s">
+      <c r="B16" s="66" t="s">
         <v>71</v>
       </c>
-      <c r="C16" s="62"/>
-      <c r="D16" s="62"/>
-      <c r="E16" s="62"/>
-      <c r="F16" s="62"/>
-      <c r="G16" s="62"/>
-      <c r="H16" s="62"/>
-      <c r="I16" s="62"/>
-      <c r="J16" s="62"/>
-      <c r="K16" s="62"/>
-      <c r="L16" s="62"/>
-      <c r="M16" s="62"/>
-      <c r="N16" s="63"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="67"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="67"/>
+      <c r="I16" s="67"/>
+      <c r="J16" s="67"/>
+      <c r="K16" s="67"/>
+      <c r="L16" s="67"/>
+      <c r="M16" s="67"/>
+      <c r="N16" s="68"/>
     </row>
     <row r="17" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1"/>
@@ -1580,21 +1571,21 @@
     </row>
     <row r="21" spans="1:14" ht="16" x14ac:dyDescent="0.15">
       <c r="A21" s="1"/>
-      <c r="B21" s="61" t="s">
+      <c r="B21" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="62"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="62"/>
-      <c r="F21" s="62"/>
-      <c r="G21" s="62"/>
-      <c r="H21" s="62"/>
-      <c r="I21" s="62"/>
-      <c r="J21" s="62"/>
-      <c r="K21" s="62"/>
-      <c r="L21" s="62"/>
-      <c r="M21" s="62"/>
-      <c r="N21" s="63"/>
+      <c r="C21" s="67"/>
+      <c r="D21" s="67"/>
+      <c r="E21" s="67"/>
+      <c r="F21" s="67"/>
+      <c r="G21" s="67"/>
+      <c r="H21" s="67"/>
+      <c r="I21" s="67"/>
+      <c r="J21" s="67"/>
+      <c r="K21" s="67"/>
+      <c r="L21" s="67"/>
+      <c r="M21" s="67"/>
+      <c r="N21" s="68"/>
     </row>
     <row r="22" spans="1:14" ht="28" x14ac:dyDescent="0.15">
       <c r="A22" s="1"/>
@@ -1662,39 +1653,39 @@
     </row>
     <row r="25" spans="1:14" ht="16" x14ac:dyDescent="0.15">
       <c r="A25" s="1"/>
-      <c r="B25" s="59" t="s">
+      <c r="B25" s="65" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="59"/>
-      <c r="D25" s="59"/>
-      <c r="E25" s="59"/>
-      <c r="F25" s="59"/>
-      <c r="G25" s="59"/>
-      <c r="H25" s="59"/>
-      <c r="I25" s="59"/>
-      <c r="J25" s="59"/>
-      <c r="K25" s="59"/>
-      <c r="L25" s="59"/>
-      <c r="M25" s="59"/>
-      <c r="N25" s="59"/>
+      <c r="C25" s="65"/>
+      <c r="D25" s="65"/>
+      <c r="E25" s="65"/>
+      <c r="F25" s="65"/>
+      <c r="G25" s="65"/>
+      <c r="H25" s="65"/>
+      <c r="I25" s="65"/>
+      <c r="J25" s="65"/>
+      <c r="K25" s="65"/>
+      <c r="L25" s="65"/>
+      <c r="M25" s="65"/>
+      <c r="N25" s="65"/>
     </row>
     <row r="26" spans="1:14" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1"/>
-      <c r="B26" s="60" t="s">
+      <c r="B26" s="81" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="60"/>
-      <c r="D26" s="60"/>
-      <c r="E26" s="60"/>
-      <c r="F26" s="60"/>
-      <c r="G26" s="60"/>
-      <c r="H26" s="60"/>
-      <c r="I26" s="60"/>
-      <c r="J26" s="60"/>
-      <c r="K26" s="60"/>
-      <c r="L26" s="60"/>
-      <c r="M26" s="60"/>
-      <c r="N26" s="60"/>
+      <c r="C26" s="82"/>
+      <c r="D26" s="82"/>
+      <c r="E26" s="82"/>
+      <c r="F26" s="82"/>
+      <c r="G26" s="82"/>
+      <c r="H26" s="82"/>
+      <c r="I26" s="82"/>
+      <c r="J26" s="82"/>
+      <c r="K26" s="82"/>
+      <c r="L26" s="82"/>
+      <c r="M26" s="82"/>
+      <c r="N26" s="83"/>
     </row>
     <row r="27" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A27" s="1"/>
@@ -1714,20 +1705,20 @@
     </row>
     <row r="28" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A28" s="1"/>
-      <c r="B28" s="48"/>
-      <c r="C28" s="49"/>
-      <c r="D28" s="49"/>
-      <c r="E28" s="49"/>
-      <c r="F28" s="49"/>
-      <c r="G28" s="50"/>
-      <c r="H28" s="56" t="s">
+      <c r="B28" s="69"/>
+      <c r="C28" s="70"/>
+      <c r="D28" s="70"/>
+      <c r="E28" s="70"/>
+      <c r="F28" s="70"/>
+      <c r="G28" s="71"/>
+      <c r="H28" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="I28" s="56"/>
-      <c r="J28" s="56" t="s">
+      <c r="I28" s="51"/>
+      <c r="J28" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="K28" s="56"/>
+      <c r="K28" s="51"/>
       <c r="L28" s="33" t="s">
         <v>20</v>
       </c>
@@ -1740,20 +1731,20 @@
     </row>
     <row r="29" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A29" s="1"/>
-      <c r="B29" s="53"/>
-      <c r="C29" s="54"/>
-      <c r="D29" s="54"/>
-      <c r="E29" s="54"/>
-      <c r="F29" s="54"/>
-      <c r="G29" s="55"/>
-      <c r="H29" s="57" t="s">
+      <c r="B29" s="74"/>
+      <c r="C29" s="75"/>
+      <c r="D29" s="75"/>
+      <c r="E29" s="75"/>
+      <c r="F29" s="75"/>
+      <c r="G29" s="76"/>
+      <c r="H29" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="I29" s="57"/>
-      <c r="J29" s="57" t="s">
+      <c r="I29" s="52"/>
+      <c r="J29" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="K29" s="57"/>
+      <c r="K29" s="52"/>
       <c r="L29" s="34" t="s">
         <v>46</v>
       </c>
@@ -1766,18 +1757,18 @@
     </row>
     <row r="30" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A30" s="1"/>
-      <c r="B30" s="51" t="s">
+      <c r="B30" s="72" t="s">
         <v>49</v>
       </c>
-      <c r="C30" s="52"/>
-      <c r="D30" s="52"/>
-      <c r="E30" s="52"/>
-      <c r="F30" s="52"/>
-      <c r="G30" s="52"/>
-      <c r="H30" s="67" t="s">
+      <c r="C30" s="73"/>
+      <c r="D30" s="73"/>
+      <c r="E30" s="73"/>
+      <c r="F30" s="73"/>
+      <c r="G30" s="73"/>
+      <c r="H30" s="79" t="s">
         <v>50</v>
       </c>
-      <c r="I30" s="68"/>
+      <c r="I30" s="80"/>
       <c r="J30" s="19"/>
       <c r="K30" s="35"/>
       <c r="L30" s="19"/>
@@ -1786,18 +1777,18 @@
     </row>
     <row r="31" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A31" s="1"/>
-      <c r="B31" s="51" t="s">
+      <c r="B31" s="72" t="s">
         <v>51</v>
       </c>
-      <c r="C31" s="52"/>
-      <c r="D31" s="52"/>
-      <c r="E31" s="52"/>
-      <c r="F31" s="52"/>
-      <c r="G31" s="52"/>
-      <c r="H31" s="67" t="s">
+      <c r="C31" s="73"/>
+      <c r="D31" s="73"/>
+      <c r="E31" s="73"/>
+      <c r="F31" s="73"/>
+      <c r="G31" s="73"/>
+      <c r="H31" s="79" t="s">
         <v>52</v>
       </c>
-      <c r="I31" s="68"/>
+      <c r="I31" s="80"/>
       <c r="J31" s="36"/>
       <c r="K31" s="35"/>
       <c r="L31" s="35"/>
@@ -1806,205 +1797,188 @@
     </row>
     <row r="32" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A32" s="1"/>
-      <c r="B32" s="51" t="s">
+      <c r="B32" s="72" t="s">
         <v>53</v>
       </c>
-      <c r="C32" s="52"/>
-      <c r="D32" s="52"/>
-      <c r="E32" s="52"/>
-      <c r="F32" s="52"/>
-      <c r="G32" s="52"/>
-      <c r="H32" s="69" t="s">
+      <c r="C32" s="73"/>
+      <c r="D32" s="73"/>
+      <c r="E32" s="73"/>
+      <c r="F32" s="73"/>
+      <c r="G32" s="73"/>
+      <c r="H32" s="58" t="s">
         <v>54</v>
       </c>
-      <c r="I32" s="70"/>
-      <c r="J32" s="70"/>
-      <c r="K32" s="70"/>
-      <c r="L32" s="70"/>
-      <c r="M32" s="70"/>
-      <c r="N32" s="71"/>
+      <c r="I32" s="59"/>
+      <c r="J32" s="59"/>
+      <c r="K32" s="59"/>
+      <c r="L32" s="59"/>
+      <c r="M32" s="59"/>
+      <c r="N32" s="60"/>
     </row>
     <row r="33" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A33" s="1"/>
-      <c r="B33" s="64"/>
-      <c r="C33" s="64"/>
-      <c r="D33" s="64"/>
-      <c r="E33" s="64"/>
-      <c r="F33" s="64"/>
-      <c r="G33" s="64"/>
-      <c r="H33" s="64"/>
-      <c r="I33" s="64"/>
-      <c r="J33" s="65"/>
-      <c r="K33" s="65"/>
-      <c r="L33" s="65"/>
-      <c r="M33" s="65"/>
-      <c r="N33" s="66"/>
+      <c r="B33" s="61"/>
+      <c r="C33" s="61"/>
+      <c r="D33" s="61"/>
+      <c r="E33" s="61"/>
+      <c r="F33" s="61"/>
+      <c r="G33" s="61"/>
+      <c r="H33" s="61"/>
+      <c r="I33" s="61"/>
+      <c r="J33" s="77"/>
+      <c r="K33" s="77"/>
+      <c r="L33" s="77"/>
+      <c r="M33" s="77"/>
+      <c r="N33" s="78"/>
     </row>
     <row r="34" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A34" s="1"/>
-      <c r="B34" s="64"/>
-      <c r="C34" s="64"/>
-      <c r="D34" s="64"/>
-      <c r="E34" s="64"/>
-      <c r="F34" s="64"/>
-      <c r="G34" s="64"/>
-      <c r="H34" s="64"/>
-      <c r="I34" s="64"/>
-      <c r="J34" s="64"/>
-      <c r="K34" s="64"/>
-      <c r="L34" s="64"/>
-      <c r="M34" s="64"/>
-      <c r="N34" s="72"/>
+      <c r="B34" s="61"/>
+      <c r="C34" s="61"/>
+      <c r="D34" s="61"/>
+      <c r="E34" s="61"/>
+      <c r="F34" s="61"/>
+      <c r="G34" s="61"/>
+      <c r="H34" s="61"/>
+      <c r="I34" s="61"/>
+      <c r="J34" s="61"/>
+      <c r="K34" s="61"/>
+      <c r="L34" s="61"/>
+      <c r="M34" s="61"/>
+      <c r="N34" s="62"/>
     </row>
     <row r="35" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="1"/>
-      <c r="B35" s="74" t="s">
+      <c r="B35" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="C35" s="57"/>
-      <c r="D35" s="57"/>
-      <c r="E35" s="57"/>
-      <c r="F35" s="57"/>
-      <c r="G35" s="57"/>
-      <c r="H35" s="57"/>
-      <c r="I35" s="57"/>
-      <c r="J35" s="57"/>
-      <c r="K35" s="57"/>
-      <c r="L35" s="57"/>
-      <c r="M35" s="57"/>
-      <c r="N35" s="75"/>
+      <c r="C35" s="52"/>
+      <c r="D35" s="52"/>
+      <c r="E35" s="52"/>
+      <c r="F35" s="52"/>
+      <c r="G35" s="52"/>
+      <c r="H35" s="52"/>
+      <c r="I35" s="52"/>
+      <c r="J35" s="52"/>
+      <c r="K35" s="52"/>
+      <c r="L35" s="52"/>
+      <c r="M35" s="52"/>
+      <c r="N35" s="53"/>
     </row>
     <row r="36" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A36" s="1"/>
-      <c r="B36" s="76" t="s">
+      <c r="B36" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="C36" s="56"/>
-      <c r="D36" s="56"/>
-      <c r="E36" s="73"/>
-      <c r="F36" s="73"/>
-      <c r="G36" s="57" t="s">
+      <c r="C36" s="51"/>
+      <c r="D36" s="51"/>
+      <c r="E36" s="47"/>
+      <c r="F36" s="47"/>
+      <c r="G36" s="52" t="s">
         <v>57</v>
       </c>
-      <c r="H36" s="57"/>
-      <c r="I36" s="57"/>
-      <c r="J36" s="57"/>
-      <c r="K36" s="57"/>
-      <c r="L36" s="57"/>
-      <c r="M36" s="57"/>
-      <c r="N36" s="75"/>
+      <c r="H36" s="52"/>
+      <c r="I36" s="52"/>
+      <c r="J36" s="52"/>
+      <c r="K36" s="52"/>
+      <c r="L36" s="52"/>
+      <c r="M36" s="52"/>
+      <c r="N36" s="53"/>
     </row>
     <row r="37" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A37" s="1"/>
-      <c r="B37" s="76" t="s">
+      <c r="B37" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="C37" s="56"/>
-      <c r="D37" s="56"/>
-      <c r="E37" s="73"/>
-      <c r="F37" s="73"/>
-      <c r="G37" s="57" t="s">
+      <c r="C37" s="51"/>
+      <c r="D37" s="51"/>
+      <c r="E37" s="47"/>
+      <c r="F37" s="47"/>
+      <c r="G37" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="H37" s="57"/>
-      <c r="I37" s="57"/>
-      <c r="J37" s="57"/>
-      <c r="K37" s="57"/>
-      <c r="L37" s="57"/>
-      <c r="M37" s="57"/>
-      <c r="N37" s="75"/>
+      <c r="H37" s="52"/>
+      <c r="I37" s="52"/>
+      <c r="J37" s="52"/>
+      <c r="K37" s="52"/>
+      <c r="L37" s="52"/>
+      <c r="M37" s="52"/>
+      <c r="N37" s="53"/>
     </row>
     <row r="38" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A38" s="1"/>
-      <c r="B38" s="76" t="s">
+      <c r="B38" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="C38" s="56"/>
-      <c r="D38" s="56"/>
-      <c r="E38" s="73"/>
-      <c r="F38" s="73"/>
-      <c r="G38" s="57" t="s">
+      <c r="C38" s="51"/>
+      <c r="D38" s="51"/>
+      <c r="E38" s="47"/>
+      <c r="F38" s="47"/>
+      <c r="G38" s="52" t="s">
         <v>61</v>
       </c>
-      <c r="H38" s="57"/>
-      <c r="I38" s="57"/>
-      <c r="J38" s="57"/>
-      <c r="K38" s="57"/>
-      <c r="L38" s="57"/>
-      <c r="M38" s="57"/>
-      <c r="N38" s="75"/>
+      <c r="H38" s="52"/>
+      <c r="I38" s="52"/>
+      <c r="J38" s="52"/>
+      <c r="K38" s="52"/>
+      <c r="L38" s="52"/>
+      <c r="M38" s="52"/>
+      <c r="N38" s="53"/>
     </row>
     <row r="39" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
-      <c r="B39" s="77" t="s">
+      <c r="B39" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="C39" s="78"/>
-      <c r="D39" s="78"/>
-      <c r="E39" s="79"/>
-      <c r="F39" s="79"/>
-      <c r="G39" s="80" t="s">
+      <c r="C39" s="55"/>
+      <c r="D39" s="55"/>
+      <c r="E39" s="48"/>
+      <c r="F39" s="48"/>
+      <c r="G39" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="H39" s="80"/>
-      <c r="I39" s="80"/>
-      <c r="J39" s="80"/>
-      <c r="K39" s="80"/>
-      <c r="L39" s="80"/>
-      <c r="M39" s="80"/>
-      <c r="N39" s="81"/>
+      <c r="H39" s="56"/>
+      <c r="I39" s="56"/>
+      <c r="J39" s="56"/>
+      <c r="K39" s="56"/>
+      <c r="L39" s="56"/>
+      <c r="M39" s="56"/>
+      <c r="N39" s="57"/>
     </row>
     <row r="40" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A40" s="1"/>
-      <c r="B40" s="47"/>
-      <c r="C40" s="47"/>
-      <c r="D40" s="47"/>
-      <c r="E40" s="47"/>
-      <c r="F40" s="47"/>
-      <c r="G40" s="47"/>
-      <c r="H40" s="47"/>
-      <c r="I40" s="47"/>
+      <c r="B40" s="49"/>
+      <c r="C40" s="49"/>
+      <c r="D40" s="49"/>
+      <c r="E40" s="49"/>
+      <c r="F40" s="49"/>
+      <c r="G40" s="49"/>
+      <c r="H40" s="49"/>
+      <c r="I40" s="49"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
     </row>
     <row r="41" spans="1:14" ht="14" x14ac:dyDescent="0.15">
-      <c r="B41" s="47" t="s">
+      <c r="B41" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="C41" s="47"/>
-      <c r="D41" s="47"/>
-      <c r="E41" s="47"/>
-      <c r="F41" s="47"/>
-      <c r="G41" s="47"/>
-      <c r="H41" s="47"/>
-      <c r="I41" s="47"/>
-      <c r="J41" s="47"/>
-      <c r="K41" s="47"/>
-      <c r="L41" s="47"/>
-      <c r="M41" s="47"/>
-      <c r="N41" s="47"/>
+      <c r="C41" s="49"/>
+      <c r="D41" s="49"/>
+      <c r="E41" s="49"/>
+      <c r="F41" s="49"/>
+      <c r="G41" s="49"/>
+      <c r="H41" s="49"/>
+      <c r="I41" s="49"/>
+      <c r="J41" s="49"/>
+      <c r="K41" s="49"/>
+      <c r="L41" s="49"/>
+      <c r="M41" s="49"/>
+      <c r="N41" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B40:I40"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="G37:N37"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="G38:N38"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="G39:N39"/>
-    <mergeCell ref="H32:N32"/>
-    <mergeCell ref="B34:N34"/>
-    <mergeCell ref="B35:N35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="G36:N36"/>
-    <mergeCell ref="B2:N2"/>
-    <mergeCell ref="B25:N25"/>
-    <mergeCell ref="B26:N26"/>
-    <mergeCell ref="B16:N16"/>
-    <mergeCell ref="B21:N21"/>
     <mergeCell ref="B41:N41"/>
     <mergeCell ref="B28:G28"/>
     <mergeCell ref="B30:G30"/>
@@ -2019,6 +1993,23 @@
     <mergeCell ref="J33:N33"/>
     <mergeCell ref="H30:I30"/>
     <mergeCell ref="H31:I31"/>
+    <mergeCell ref="B2:N2"/>
+    <mergeCell ref="B25:N25"/>
+    <mergeCell ref="B26:N26"/>
+    <mergeCell ref="B16:N16"/>
+    <mergeCell ref="B21:N21"/>
+    <mergeCell ref="H32:N32"/>
+    <mergeCell ref="B34:N34"/>
+    <mergeCell ref="B35:N35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="G36:N36"/>
+    <mergeCell ref="B40:I40"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="G37:N37"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="G38:N38"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="G39:N39"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
CRM-3513 Make SF template dynamic make main company detail dynamic as per kenstar requirement
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Vendor_Settlement_Template-FoC-v4.xlsx
+++ b/application/controllers/excel-templates/Vendor_Settlement_Template-FoC-v4.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\247around-adminp-aws\application\controllers\excel-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B83157-0B23-4035-8AF4-E0A8ACE8D534}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A1ACA3-421E-4E6C-AAA7-D626F9DBC0B4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,15 +49,6 @@
     <t>BILL TO:</t>
   </si>
   <si>
-    <t>Blackmelon Advance Technology Co. Pvt. Ltd.</t>
-  </si>
-  <si>
-    <t>Delhi - 110051</t>
-  </si>
-  <si>
-    <t>GSTIN: 07AAFCB1281J1ZQ</t>
-  </si>
-  <si>
     <t>Installation Details</t>
   </si>
   <si>
@@ -262,7 +253,16 @@
     <t>{meta:ifsc_code}</t>
   </si>
   <si>
-    <t xml:space="preserve">A-1/7, F/F A BLOCK, KRISHNA NAGAR, </t>
+    <t>{meta:main_company_name}</t>
+  </si>
+  <si>
+    <t>{meta:main_company_address},</t>
+  </si>
+  <si>
+    <t>{meta:main_company_state} - {meta:main_company_pincode}</t>
+  </si>
+  <si>
+    <t>GSTIN: {meta:main_company_gst_number}</t>
   </si>
 </sst>
 </file>
@@ -716,60 +716,60 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1089,7 +1089,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1116,19 +1116,19 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="50"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -1248,7 +1248,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>9</v>
+        <v>77</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1264,7 +1264,7 @@
       <c r="A11" s="1"/>
       <c r="B11" s="14"/>
       <c r="C11" s="16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1280,7 +1280,7 @@
       <c r="A12" s="1"/>
       <c r="B12" s="17"/>
       <c r="C12" s="16" t="s">
-        <v>10</v>
+        <v>79</v>
       </c>
       <c r="D12" s="18"/>
       <c r="E12" s="18"/>
@@ -1296,7 +1296,7 @@
       <c r="A13" s="1"/>
       <c r="B13" s="17"/>
       <c r="C13" s="19" t="s">
-        <v>11</v>
+        <v>80</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
@@ -1338,8 +1338,8 @@
     </row>
     <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="53" t="s">
-        <v>12</v>
+      <c r="B16" s="52" t="s">
+        <v>9</v>
       </c>
       <c r="C16" s="40"/>
       <c r="D16" s="40"/>
@@ -1355,73 +1355,73 @@
     <row r="17" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="F17" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="G17" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="22" t="s">
+      <c r="H17" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F17" s="22" t="s">
+      <c r="I17" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="G17" s="20" t="s">
+      <c r="J17" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H17" s="20" t="s">
+      <c r="K17" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I17" s="23" t="s">
+      <c r="L17" s="20" t="s">
         <v>20</v>
-      </c>
-      <c r="J17" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="K17" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="L17" s="20" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="F18" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="24" t="s">
+      <c r="G18" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="24" t="s">
+      <c r="H18" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="24" t="s">
+      <c r="I18" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="G18" s="24" t="s">
+      <c r="J18" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="H18" s="24" t="s">
+      <c r="K18" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="I18" s="24" t="s">
+      <c r="L18" s="24" t="s">
         <v>31</v>
-      </c>
-      <c r="J18" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="K18" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="L18" s="24" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1454,8 +1454,8 @@
     </row>
     <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="53" t="s">
-        <v>35</v>
+      <c r="B21" s="52" t="s">
+        <v>32</v>
       </c>
       <c r="C21" s="40"/>
       <c r="D21" s="40"/>
@@ -1471,21 +1471,21 @@
     <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="25" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="D22" s="47" t="s">
-        <v>37</v>
+        <v>33</v>
+      </c>
+      <c r="D22" s="45" t="s">
+        <v>34</v>
       </c>
       <c r="E22" s="40"/>
       <c r="F22" s="41"/>
       <c r="G22" s="25" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H22" s="25" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I22" s="26"/>
       <c r="J22" s="26"/>
@@ -1495,21 +1495,21 @@
     <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="24" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="45" t="s">
-        <v>41</v>
+        <v>37</v>
+      </c>
+      <c r="D23" s="39" t="s">
+        <v>38</v>
       </c>
       <c r="E23" s="40"/>
       <c r="F23" s="41"/>
       <c r="G23" s="24" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H23" s="24" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I23" s="26"/>
       <c r="J23" s="26"/>
@@ -1532,8 +1532,8 @@
     </row>
     <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-      <c r="B25" s="53" t="s">
-        <v>44</v>
+      <c r="B25" s="52" t="s">
+        <v>41</v>
       </c>
       <c r="C25" s="40"/>
       <c r="D25" s="40"/>
@@ -1549,21 +1549,21 @@
     <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="25" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="D26" s="47" t="s">
-        <v>37</v>
+        <v>33</v>
+      </c>
+      <c r="D26" s="45" t="s">
+        <v>34</v>
       </c>
       <c r="E26" s="40"/>
       <c r="F26" s="41"/>
       <c r="G26" s="25" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H26" s="25" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I26" s="26"/>
       <c r="J26" s="26"/>
@@ -1573,21 +1573,21 @@
     <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="24" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="D27" s="45" t="s">
-        <v>47</v>
+        <v>43</v>
+      </c>
+      <c r="D27" s="39" t="s">
+        <v>44</v>
       </c>
       <c r="E27" s="40"/>
       <c r="F27" s="41"/>
       <c r="G27" s="24" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H27" s="24" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I27" s="26"/>
       <c r="J27" s="26"/>
@@ -1610,8 +1610,8 @@
     </row>
     <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
-      <c r="B29" s="53" t="s">
-        <v>50</v>
+      <c r="B29" s="52" t="s">
+        <v>47</v>
       </c>
       <c r="C29" s="40"/>
       <c r="D29" s="40"/>
@@ -1627,10 +1627,10 @@
     <row r="30" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="25" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
@@ -1645,10 +1645,10 @@
     <row r="31" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="24" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
@@ -1662,24 +1662,24 @@
     </row>
     <row r="32" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
-      <c r="B32" s="54" t="s">
-        <v>53</v>
-      </c>
-      <c r="C32" s="43"/>
-      <c r="D32" s="43"/>
-      <c r="E32" s="43"/>
-      <c r="F32" s="43"/>
-      <c r="G32" s="43"/>
-      <c r="H32" s="43"/>
-      <c r="I32" s="43"/>
-      <c r="J32" s="43"/>
-      <c r="K32" s="43"/>
+      <c r="B32" s="53" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" s="54"/>
+      <c r="D32" s="54"/>
+      <c r="E32" s="54"/>
+      <c r="F32" s="54"/>
+      <c r="G32" s="54"/>
+      <c r="H32" s="54"/>
+      <c r="I32" s="54"/>
+      <c r="J32" s="54"/>
+      <c r="K32" s="54"/>
       <c r="L32" s="55"/>
     </row>
     <row r="33" spans="1:26" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
-      <c r="B33" s="57" t="s">
-        <v>54</v>
+      <c r="B33" s="58" t="s">
+        <v>51</v>
       </c>
       <c r="C33" s="40"/>
       <c r="D33" s="40"/>
@@ -1708,58 +1708,58 @@
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
-      <c r="B35" s="58"/>
-      <c r="C35" s="50"/>
-      <c r="D35" s="50"/>
-      <c r="E35" s="50"/>
-      <c r="F35" s="50"/>
-      <c r="G35" s="50"/>
-      <c r="H35" s="47" t="s">
-        <v>20</v>
+      <c r="B35" s="46"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="43"/>
+      <c r="E35" s="43"/>
+      <c r="F35" s="43"/>
+      <c r="G35" s="43"/>
+      <c r="H35" s="45" t="s">
+        <v>17</v>
       </c>
       <c r="I35" s="41"/>
-      <c r="J35" s="47" t="s">
-        <v>21</v>
+      <c r="J35" s="45" t="s">
+        <v>18</v>
       </c>
       <c r="K35" s="41"/>
       <c r="L35" s="25" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
-      <c r="B36" s="58"/>
-      <c r="C36" s="50"/>
-      <c r="D36" s="50"/>
-      <c r="E36" s="50"/>
-      <c r="F36" s="50"/>
-      <c r="G36" s="50"/>
-      <c r="H36" s="45" t="s">
-        <v>55</v>
+      <c r="B36" s="46"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="43"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="43"/>
+      <c r="H36" s="39" t="s">
+        <v>52</v>
       </c>
       <c r="I36" s="41"/>
-      <c r="J36" s="45" t="s">
-        <v>56</v>
+      <c r="J36" s="39" t="s">
+        <v>53</v>
       </c>
       <c r="K36" s="41"/>
       <c r="L36" s="24" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
-      <c r="B37" s="39" t="s">
-        <v>50</v>
+      <c r="B37" s="51" t="s">
+        <v>47</v>
       </c>
       <c r="C37" s="40"/>
       <c r="D37" s="40"/>
       <c r="E37" s="40"/>
       <c r="F37" s="40"/>
       <c r="G37" s="41"/>
-      <c r="H37" s="45" t="s">
-        <v>58</v>
-      </c>
-      <c r="I37" s="48"/>
+      <c r="H37" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="I37" s="56"/>
       <c r="J37" s="28"/>
       <c r="K37" s="29"/>
       <c r="L37" s="30"/>
@@ -1780,144 +1780,144 @@
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
-      <c r="B38" s="39" t="s">
-        <v>59</v>
+      <c r="B38" s="51" t="s">
+        <v>56</v>
       </c>
       <c r="C38" s="40"/>
       <c r="D38" s="40"/>
       <c r="E38" s="40"/>
       <c r="F38" s="40"/>
       <c r="G38" s="41"/>
-      <c r="H38" s="45" t="s">
-        <v>60</v>
-      </c>
-      <c r="I38" s="48"/>
+      <c r="H38" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="I38" s="56"/>
       <c r="J38" s="32"/>
       <c r="K38" s="33"/>
       <c r="L38" s="34"/>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
-      <c r="B39" s="39" t="s">
-        <v>61</v>
+      <c r="B39" s="51" t="s">
+        <v>58</v>
       </c>
       <c r="C39" s="40"/>
       <c r="D39" s="40"/>
       <c r="E39" s="40"/>
       <c r="F39" s="40"/>
       <c r="G39" s="41"/>
-      <c r="H39" s="52" t="s">
-        <v>62</v>
-      </c>
-      <c r="I39" s="44"/>
+      <c r="H39" s="60" t="s">
+        <v>59</v>
+      </c>
+      <c r="I39" s="61"/>
       <c r="J39" s="32"/>
       <c r="K39" s="33"/>
       <c r="L39" s="34"/>
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="35"/>
-      <c r="B40" s="42" t="s">
-        <v>63</v>
-      </c>
-      <c r="C40" s="43"/>
-      <c r="D40" s="43"/>
-      <c r="E40" s="43"/>
-      <c r="F40" s="43"/>
-      <c r="G40" s="44"/>
-      <c r="H40" s="52" t="s">
-        <v>64</v>
-      </c>
-      <c r="I40" s="44"/>
+      <c r="B40" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="C40" s="54"/>
+      <c r="D40" s="54"/>
+      <c r="E40" s="54"/>
+      <c r="F40" s="54"/>
+      <c r="G40" s="61"/>
+      <c r="H40" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="I40" s="61"/>
       <c r="J40" s="29"/>
       <c r="K40" s="36"/>
       <c r="L40" s="37"/>
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="35"/>
-      <c r="B41" s="39" t="s">
-        <v>65</v>
+      <c r="B41" s="51" t="s">
+        <v>62</v>
       </c>
       <c r="C41" s="40"/>
       <c r="D41" s="40"/>
       <c r="E41" s="40"/>
       <c r="F41" s="40"/>
       <c r="G41" s="41"/>
-      <c r="H41" s="45" t="s">
-        <v>66</v>
-      </c>
-      <c r="I41" s="48"/>
+      <c r="H41" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="I41" s="56"/>
       <c r="J41" s="29"/>
       <c r="K41" s="36"/>
       <c r="L41" s="37"/>
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
-      <c r="B42" s="59" t="s">
-        <v>67</v>
-      </c>
-      <c r="C42" s="60"/>
-      <c r="D42" s="60"/>
-      <c r="E42" s="60"/>
-      <c r="F42" s="60"/>
-      <c r="G42" s="61"/>
-      <c r="H42" s="62" t="s">
-        <v>68</v>
-      </c>
-      <c r="I42" s="63"/>
+      <c r="B42" s="62" t="s">
+        <v>64</v>
+      </c>
+      <c r="C42" s="49"/>
+      <c r="D42" s="49"/>
+      <c r="E42" s="49"/>
+      <c r="F42" s="49"/>
+      <c r="G42" s="50"/>
+      <c r="H42" s="63" t="s">
+        <v>65</v>
+      </c>
+      <c r="I42" s="64"/>
       <c r="J42" s="32"/>
       <c r="K42" s="33"/>
       <c r="L42" s="34"/>
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
-      <c r="B43" s="39" t="s">
-        <v>69</v>
+      <c r="B43" s="51" t="s">
+        <v>66</v>
       </c>
       <c r="C43" s="40"/>
       <c r="D43" s="40"/>
       <c r="E43" s="40"/>
       <c r="F43" s="40"/>
       <c r="G43" s="41"/>
-      <c r="H43" s="66" t="s">
-        <v>70</v>
-      </c>
-      <c r="I43" s="60"/>
-      <c r="J43" s="60"/>
-      <c r="K43" s="60"/>
-      <c r="L43" s="61"/>
+      <c r="H43" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="I43" s="49"/>
+      <c r="J43" s="49"/>
+      <c r="K43" s="49"/>
+      <c r="L43" s="50"/>
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
-      <c r="B44" s="58"/>
-      <c r="C44" s="50"/>
-      <c r="D44" s="50"/>
-      <c r="E44" s="50"/>
-      <c r="F44" s="50"/>
-      <c r="G44" s="50"/>
-      <c r="H44" s="50"/>
-      <c r="I44" s="50"/>
-      <c r="J44" s="49"/>
-      <c r="K44" s="50"/>
-      <c r="L44" s="51"/>
+      <c r="B44" s="46"/>
+      <c r="C44" s="43"/>
+      <c r="D44" s="43"/>
+      <c r="E44" s="43"/>
+      <c r="F44" s="43"/>
+      <c r="G44" s="43"/>
+      <c r="H44" s="43"/>
+      <c r="I44" s="43"/>
+      <c r="J44" s="59"/>
+      <c r="K44" s="43"/>
+      <c r="L44" s="47"/>
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
-      <c r="B45" s="58"/>
-      <c r="C45" s="50"/>
-      <c r="D45" s="50"/>
-      <c r="E45" s="50"/>
-      <c r="F45" s="50"/>
-      <c r="G45" s="50"/>
-      <c r="H45" s="50"/>
-      <c r="I45" s="50"/>
-      <c r="J45" s="50"/>
-      <c r="K45" s="50"/>
-      <c r="L45" s="51"/>
+      <c r="B45" s="46"/>
+      <c r="C45" s="43"/>
+      <c r="D45" s="43"/>
+      <c r="E45" s="43"/>
+      <c r="F45" s="43"/>
+      <c r="G45" s="43"/>
+      <c r="H45" s="43"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
+      <c r="K45" s="43"/>
+      <c r="L45" s="47"/>
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
-      <c r="B46" s="45" t="s">
-        <v>71</v>
+      <c r="B46" s="39" t="s">
+        <v>68</v>
       </c>
       <c r="C46" s="40"/>
       <c r="D46" s="40"/>
@@ -1932,15 +1932,15 @@
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
-      <c r="B47" s="47" t="s">
-        <v>72</v>
+      <c r="B47" s="45" t="s">
+        <v>69</v>
       </c>
       <c r="C47" s="40"/>
       <c r="D47" s="41"/>
       <c r="E47" s="38"/>
       <c r="F47" s="38"/>
-      <c r="G47" s="45" t="s">
-        <v>73</v>
+      <c r="G47" s="39" t="s">
+        <v>70</v>
       </c>
       <c r="H47" s="40"/>
       <c r="I47" s="40"/>
@@ -1950,15 +1950,15 @@
     </row>
     <row r="48" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
-      <c r="B48" s="47" t="s">
-        <v>74</v>
+      <c r="B48" s="45" t="s">
+        <v>71</v>
       </c>
       <c r="C48" s="40"/>
       <c r="D48" s="41"/>
       <c r="E48" s="38"/>
       <c r="F48" s="38"/>
-      <c r="G48" s="46" t="s">
-        <v>75</v>
+      <c r="G48" s="66" t="s">
+        <v>72</v>
       </c>
       <c r="H48" s="40"/>
       <c r="I48" s="40"/>
@@ -1968,15 +1968,15 @@
     </row>
     <row r="49" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
-      <c r="B49" s="47" t="s">
-        <v>76</v>
+      <c r="B49" s="45" t="s">
+        <v>73</v>
       </c>
       <c r="C49" s="40"/>
       <c r="D49" s="41"/>
       <c r="E49" s="38"/>
       <c r="F49" s="38"/>
-      <c r="G49" s="45" t="s">
-        <v>77</v>
+      <c r="G49" s="39" t="s">
+        <v>74</v>
       </c>
       <c r="H49" s="40"/>
       <c r="I49" s="40"/>
@@ -1986,15 +1986,15 @@
     </row>
     <row r="50" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
-      <c r="B50" s="47" t="s">
-        <v>78</v>
+      <c r="B50" s="45" t="s">
+        <v>75</v>
       </c>
       <c r="C50" s="40"/>
       <c r="D50" s="41"/>
       <c r="E50" s="38"/>
       <c r="F50" s="38"/>
-      <c r="G50" s="45" t="s">
-        <v>79</v>
+      <c r="G50" s="39" t="s">
+        <v>76</v>
       </c>
       <c r="H50" s="40"/>
       <c r="I50" s="40"/>
@@ -2004,31 +2004,31 @@
     </row>
     <row r="51" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
-      <c r="B51" s="65"/>
-      <c r="C51" s="50"/>
-      <c r="D51" s="50"/>
-      <c r="E51" s="50"/>
-      <c r="F51" s="50"/>
-      <c r="G51" s="50"/>
-      <c r="H51" s="50"/>
-      <c r="I51" s="50"/>
+      <c r="B51" s="44"/>
+      <c r="C51" s="43"/>
+      <c r="D51" s="43"/>
+      <c r="E51" s="43"/>
+      <c r="F51" s="43"/>
+      <c r="G51" s="43"/>
+      <c r="H51" s="43"/>
+      <c r="I51" s="43"/>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
     </row>
     <row r="52" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
-      <c r="B52" s="64"/>
-      <c r="C52" s="50"/>
-      <c r="D52" s="50"/>
-      <c r="E52" s="50"/>
-      <c r="F52" s="50"/>
-      <c r="G52" s="50"/>
-      <c r="H52" s="50"/>
-      <c r="I52" s="50"/>
-      <c r="J52" s="50"/>
-      <c r="K52" s="50"/>
-      <c r="L52" s="50"/>
+      <c r="B52" s="42"/>
+      <c r="C52" s="43"/>
+      <c r="D52" s="43"/>
+      <c r="E52" s="43"/>
+      <c r="F52" s="43"/>
+      <c r="G52" s="43"/>
+      <c r="H52" s="43"/>
+      <c r="I52" s="43"/>
+      <c r="J52" s="43"/>
+      <c r="K52" s="43"/>
+      <c r="L52" s="43"/>
     </row>
     <row r="53" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="54" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2980,27 +2980,14 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="B52:L52"/>
-    <mergeCell ref="B51:I51"/>
-    <mergeCell ref="J35:K35"/>
-    <mergeCell ref="B45:L45"/>
-    <mergeCell ref="H43:L43"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="J36:K36"/>
-    <mergeCell ref="B29:L29"/>
-    <mergeCell ref="B32:L32"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="B16:L16"/>
-    <mergeCell ref="B21:L21"/>
-    <mergeCell ref="B33:L33"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B36:G36"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="B39:G39"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="B41:G41"/>
+    <mergeCell ref="G49:L49"/>
+    <mergeCell ref="G48:L48"/>
+    <mergeCell ref="G47:L47"/>
+    <mergeCell ref="B46:L46"/>
     <mergeCell ref="H36:I36"/>
     <mergeCell ref="B25:L25"/>
     <mergeCell ref="D26:F26"/>
@@ -3017,14 +3004,27 @@
     <mergeCell ref="B43:G43"/>
     <mergeCell ref="B47:D47"/>
     <mergeCell ref="B48:D48"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="B39:G39"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="B41:G41"/>
-    <mergeCell ref="G49:L49"/>
-    <mergeCell ref="G48:L48"/>
-    <mergeCell ref="G47:L47"/>
-    <mergeCell ref="B46:L46"/>
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B16:L16"/>
+    <mergeCell ref="B21:L21"/>
+    <mergeCell ref="B33:L33"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="B52:L52"/>
+    <mergeCell ref="B51:I51"/>
+    <mergeCell ref="J35:K35"/>
+    <mergeCell ref="B45:L45"/>
+    <mergeCell ref="H43:L43"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="B29:L29"/>
+    <mergeCell ref="B32:L32"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B36:G36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Show Sepearte Miscellaneous charges in the FOC invoice #CRM-5629
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Vendor_Settlement_Template-FoC-v4.xlsx
+++ b/application/controllers/excel-templates/Vendor_Settlement_Template-FoC-v4.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="83">
   <si>
     <t>ANNEXURE</t>
   </si>
@@ -181,7 +181,16 @@
     <t>{meta:msg}</t>
   </si>
   <si>
+    <t>Miscellaneous Charges</t>
+  </si>
+  <si>
+    <t>Parts Charge</t>
+  </si>
+  <si>
     <t>{meta:t_ic}</t>
+  </si>
+  <si>
+    <t>{meta:miscellaneous_charges}</t>
   </si>
   <si>
     <t>{meta:t_stand}</t>
@@ -257,21 +266,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="9">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10.0"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <b/>
       <sz val="14.0"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Cambria"/>
     </font>
     <font>
@@ -282,27 +286,16 @@
     </font>
     <font>
       <sz val="10.0"/>
-      <color theme="1"/>
-      <name val="Cambria"/>
-    </font>
-    <font>
-      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
     </font>
     <font>
       <b/>
       <sz val="12.0"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Cambria"/>
     </font>
     <font/>
-    <font>
-      <b/>
-      <sz val="12.0"/>
-      <color rgb="FF000000"/>
-      <name val="Cambria"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -548,173 +541,173 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="3" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="3" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="6" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="3" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="6" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="7" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="5" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="6" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="6" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="6" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="7" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="5" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="5" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="5" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="6" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="10" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="10" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="11" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="4" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="4" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="11" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="12" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="12" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="12" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="12" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="8" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="12" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="13" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="8" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="14" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="15" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="8" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="7" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="16" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="17" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="18" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="13" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="14" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="15" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="8" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="16" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="8" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="17" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="18" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="19" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="19" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="18" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="18" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="19" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="19" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="13" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="13" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="20" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="20" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="13" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="18" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="13" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="19" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="21" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="18" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="19" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="21" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="22" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="23" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="21" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="24" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="22" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="23" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="21" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="25" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="24" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="21" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="25" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="12" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="8" fillId="2" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="8" fillId="2" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -1543,27 +1536,31 @@
       </c>
       <c r="I35" s="23"/>
       <c r="J35" s="30" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="K35" s="23"/>
-      <c r="L35" s="29"/>
+      <c r="L35" s="29" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="1"/>
       <c r="B36" s="38"/>
       <c r="H36" s="32" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I36" s="23"/>
-      <c r="J36" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="K36" s="23"/>
-      <c r="L36" s="28"/>
+      <c r="J36" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="L36" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="M36" s="23"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="1"/>
-      <c r="B37" s="39" t="s">
+      <c r="B37" s="40" t="s">
         <v>51</v>
       </c>
       <c r="C37" s="22"/>
@@ -1572,31 +1569,31 @@
       <c r="F37" s="22"/>
       <c r="G37" s="23"/>
       <c r="H37" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="I37" s="40"/>
-      <c r="J37" s="41"/>
-      <c r="K37" s="42"/>
-      <c r="L37" s="43"/>
-      <c r="M37" s="44"/>
-      <c r="N37" s="44"/>
-      <c r="O37" s="44"/>
-      <c r="P37" s="44"/>
-      <c r="Q37" s="44"/>
-      <c r="R37" s="44"/>
-      <c r="S37" s="44"/>
-      <c r="T37" s="44"/>
-      <c r="U37" s="44"/>
-      <c r="V37" s="44"/>
-      <c r="W37" s="44"/>
-      <c r="X37" s="44"/>
-      <c r="Y37" s="44"/>
-      <c r="Z37" s="44"/>
+        <v>61</v>
+      </c>
+      <c r="I37" s="41"/>
+      <c r="J37" s="42"/>
+      <c r="K37" s="43"/>
+      <c r="L37" s="44"/>
+      <c r="M37" s="45"/>
+      <c r="N37" s="45"/>
+      <c r="O37" s="45"/>
+      <c r="P37" s="45"/>
+      <c r="Q37" s="45"/>
+      <c r="R37" s="45"/>
+      <c r="S37" s="45"/>
+      <c r="T37" s="45"/>
+      <c r="U37" s="45"/>
+      <c r="V37" s="45"/>
+      <c r="W37" s="45"/>
+      <c r="X37" s="45"/>
+      <c r="Y37" s="45"/>
+      <c r="Z37" s="45"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="1"/>
-      <c r="B38" s="39" t="s">
-        <v>59</v>
+      <c r="B38" s="40" t="s">
+        <v>62</v>
       </c>
       <c r="C38" s="22"/>
       <c r="D38" s="22"/>
@@ -1604,53 +1601,53 @@
       <c r="F38" s="22"/>
       <c r="G38" s="23"/>
       <c r="H38" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="I38" s="40"/>
-      <c r="J38" s="45"/>
-      <c r="K38" s="46"/>
-      <c r="L38" s="47"/>
+        <v>63</v>
+      </c>
+      <c r="I38" s="41"/>
+      <c r="J38" s="46"/>
+      <c r="K38" s="47"/>
+      <c r="L38" s="48"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="1"/>
-      <c r="B39" s="39" t="s">
-        <v>61</v>
+      <c r="B39" s="40" t="s">
+        <v>64</v>
       </c>
       <c r="C39" s="22"/>
       <c r="D39" s="22"/>
       <c r="E39" s="22"/>
       <c r="F39" s="22"/>
       <c r="G39" s="23"/>
-      <c r="H39" s="48" t="s">
-        <v>62</v>
-      </c>
-      <c r="I39" s="49"/>
-      <c r="J39" s="45"/>
-      <c r="K39" s="46"/>
-      <c r="L39" s="47"/>
+      <c r="H39" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="I39" s="50"/>
+      <c r="J39" s="46"/>
+      <c r="K39" s="47"/>
+      <c r="L39" s="48"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="50"/>
+      <c r="A40" s="45"/>
       <c r="B40" s="51" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C40" s="34"/>
       <c r="D40" s="34"/>
       <c r="E40" s="34"/>
       <c r="F40" s="34"/>
-      <c r="G40" s="49"/>
-      <c r="H40" s="48" t="s">
-        <v>64</v>
-      </c>
-      <c r="I40" s="49"/>
-      <c r="J40" s="42"/>
+      <c r="G40" s="50"/>
+      <c r="H40" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="I40" s="50"/>
+      <c r="J40" s="43"/>
       <c r="K40" s="52"/>
       <c r="L40" s="53"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="50"/>
-      <c r="B41" s="39" t="s">
-        <v>65</v>
+      <c r="A41" s="45"/>
+      <c r="B41" s="40" t="s">
+        <v>68</v>
       </c>
       <c r="C41" s="22"/>
       <c r="D41" s="22"/>
@@ -1658,17 +1655,17 @@
       <c r="F41" s="22"/>
       <c r="G41" s="23"/>
       <c r="H41" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="I41" s="40"/>
-      <c r="J41" s="42"/>
+        <v>69</v>
+      </c>
+      <c r="I41" s="41"/>
+      <c r="J41" s="43"/>
       <c r="K41" s="52"/>
       <c r="L41" s="53"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="1"/>
       <c r="B42" s="54" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C42" s="55"/>
       <c r="D42" s="55"/>
@@ -1676,17 +1673,17 @@
       <c r="F42" s="55"/>
       <c r="G42" s="56"/>
       <c r="H42" s="57" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="I42" s="58"/>
-      <c r="J42" s="45"/>
-      <c r="K42" s="46"/>
-      <c r="L42" s="47"/>
+      <c r="J42" s="46"/>
+      <c r="K42" s="47"/>
+      <c r="L42" s="48"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="1"/>
-      <c r="B43" s="39" t="s">
-        <v>69</v>
+      <c r="B43" s="40" t="s">
+        <v>72</v>
       </c>
       <c r="C43" s="22"/>
       <c r="D43" s="22"/>
@@ -1694,7 +1691,7 @@
       <c r="F43" s="22"/>
       <c r="G43" s="23"/>
       <c r="H43" s="59" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="I43" s="55"/>
       <c r="J43" s="55"/>
@@ -1704,7 +1701,7 @@
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="1"/>
       <c r="B44" s="38"/>
-      <c r="J44" s="50"/>
+      <c r="J44" s="45"/>
       <c r="L44" s="60"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
@@ -1715,7 +1712,7 @@
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="1"/>
       <c r="B46" s="32" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C46" s="22"/>
       <c r="D46" s="22"/>
@@ -1731,14 +1728,14 @@
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="1"/>
       <c r="B47" s="30" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C47" s="22"/>
       <c r="D47" s="23"/>
       <c r="E47" s="61"/>
       <c r="F47" s="61"/>
       <c r="G47" s="32" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="H47" s="22"/>
       <c r="I47" s="22"/>
@@ -1749,14 +1746,14 @@
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="1"/>
       <c r="B48" s="30" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C48" s="22"/>
       <c r="D48" s="23"/>
       <c r="E48" s="61"/>
       <c r="F48" s="61"/>
       <c r="G48" s="62" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H48" s="22"/>
       <c r="I48" s="22"/>
@@ -1767,14 +1764,14 @@
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="1"/>
       <c r="B49" s="30" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C49" s="22"/>
       <c r="D49" s="23"/>
       <c r="E49" s="61"/>
       <c r="F49" s="61"/>
       <c r="G49" s="32" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="H49" s="22"/>
       <c r="I49" s="22"/>
@@ -1785,14 +1782,14 @@
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="1"/>
       <c r="B50" s="30" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C50" s="22"/>
       <c r="D50" s="23"/>
       <c r="E50" s="61"/>
       <c r="F50" s="61"/>
       <c r="G50" s="32" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="H50" s="22"/>
       <c r="I50" s="22"/>
@@ -1802,7 +1799,7 @@
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="1"/>
-      <c r="B51" s="44"/>
+      <c r="B51" s="45"/>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
@@ -2760,7 +2757,7 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="45">
+  <mergeCells count="46">
     <mergeCell ref="B2:L2"/>
     <mergeCell ref="B16:L16"/>
     <mergeCell ref="B21:L21"/>
@@ -2778,34 +2775,35 @@
     <mergeCell ref="B36:G36"/>
     <mergeCell ref="H36:I36"/>
     <mergeCell ref="J36:K36"/>
+    <mergeCell ref="L36:M36"/>
     <mergeCell ref="B37:G37"/>
     <mergeCell ref="H37:I37"/>
+    <mergeCell ref="H38:I38"/>
     <mergeCell ref="B38:G38"/>
-    <mergeCell ref="H38:I38"/>
     <mergeCell ref="B39:G39"/>
     <mergeCell ref="H39:I39"/>
     <mergeCell ref="B40:G40"/>
     <mergeCell ref="H40:I40"/>
     <mergeCell ref="B41:G41"/>
     <mergeCell ref="H41:I41"/>
+    <mergeCell ref="B42:G42"/>
     <mergeCell ref="H42:I42"/>
-    <mergeCell ref="B42:G42"/>
     <mergeCell ref="B43:G43"/>
     <mergeCell ref="H43:L43"/>
     <mergeCell ref="B44:I44"/>
     <mergeCell ref="J44:L44"/>
     <mergeCell ref="B45:L45"/>
-    <mergeCell ref="B46:L46"/>
-    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="G49:L49"/>
+    <mergeCell ref="G50:L50"/>
     <mergeCell ref="B51:I51"/>
     <mergeCell ref="B52:L52"/>
+    <mergeCell ref="B46:L46"/>
     <mergeCell ref="B47:D47"/>
     <mergeCell ref="G47:L47"/>
     <mergeCell ref="B48:D48"/>
     <mergeCell ref="G48:L48"/>
     <mergeCell ref="B49:D49"/>
-    <mergeCell ref="G49:L49"/>
-    <mergeCell ref="G50:L50"/>
+    <mergeCell ref="B50:D50"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>